<commit_message>
Add Expense Ratio Buttons
Add ability to update Catalyst and Rational Expense Ratios through Datalinker.
</commit_message>
<xml_diff>
--- a/assets/ChartBuilder/public/Data/Backups/Rational/PBX/PBX.xlsx
+++ b/assets/ChartBuilder/public/Data/Backups/Rational/PBX/PBX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Marketing Team Files\Marketing Materials\AutoCharts&amp;Tables\Backup Files\Rational\PBX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E094896A-D378-4FB9-9BFC-0B609143071A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495D36E6-8F67-4A34-870F-CEDE97C3F390}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="821" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBX Return Data" sheetId="7" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="314">
   <si>
     <t>Inception*</t>
   </si>
@@ -1030,6 +1030,15 @@
   </si>
   <si>
     <t>*Inception: 03/01/2017. The performance shown prior to December 6, 2019 is that of the Predecessor Fund, which reflects all of the Predecessor Fund's actual fees and expenses adjusted to include any fees of each share class.</t>
+  </si>
+  <si>
+    <t>Convertible Bonds</t>
+  </si>
+  <si>
+    <t>Preferred Stocks</t>
+  </si>
+  <si>
+    <t>Common Stocks</t>
   </si>
 </sst>
 </file>
@@ -2350,6 +2359,21 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="9" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="20" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="20" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2379,21 +2403,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="20" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="20" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -23829,7 +23838,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -28671,7 +28680,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -28692,7 +28701,7 @@
     <row r="2" spans="1:2">
       <c r="A2" s="156" t="str">
         <f>'PBX - FACT SHEET'!N5</f>
-        <v>Conv</v>
+        <v>Convertible Bonds</v>
       </c>
       <c r="B2" s="157">
         <f>'PBX - FACT SHEET'!O5*100</f>
@@ -28702,7 +28711,7 @@
     <row r="3" spans="1:2">
       <c r="A3" s="156" t="str">
         <f>'PBX - FACT SHEET'!N6</f>
-        <v>Pfd</v>
+        <v>Preferred Stocks</v>
       </c>
       <c r="B3" s="157">
         <f>'PBX - FACT SHEET'!O6*100</f>
@@ -28722,7 +28731,7 @@
     <row r="5" spans="1:2">
       <c r="A5" s="156" t="str">
         <f>'PBX - FACT SHEET'!N8</f>
-        <v>Common</v>
+        <v>Common Stocks</v>
       </c>
       <c r="B5" s="157">
         <f>'PBX - FACT SHEET'!O8*100</f>
@@ -28744,8 +28753,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -28772,25 +28781,25 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="24" customFormat="1" ht="16.5" thickBot="1">
-      <c r="B2" s="214" t="s">
+      <c r="B2" s="219" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
-      <c r="H2" s="215"/>
-      <c r="I2" s="215"/>
-      <c r="J2" s="216"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
+      <c r="H2" s="220"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="221"/>
       <c r="L2" s="25"/>
-      <c r="M2" s="214" t="s">
+      <c r="M2" s="219" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="215"/>
-      <c r="O2" s="215"/>
-      <c r="P2" s="215"/>
-      <c r="Q2" s="216"/>
+      <c r="N2" s="220"/>
+      <c r="O2" s="220"/>
+      <c r="P2" s="220"/>
+      <c r="Q2" s="221"/>
     </row>
     <row r="3" spans="2:17" ht="15.75" thickBot="1">
       <c r="B3" s="10"/>
@@ -28808,10 +28817,10 @@
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1">
       <c r="B4" s="14"/>
-      <c r="C4" s="217" t="s">
+      <c r="C4" s="222" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="219">
+      <c r="D4" s="224">
         <f>'[5]PBX Return Data'!W2</f>
         <v>44286</v>
       </c>
@@ -28835,8 +28844,8 @@
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="14"/>
-      <c r="C5" s="218"/>
-      <c r="D5" s="220"/>
+      <c r="C5" s="223"/>
+      <c r="D5" s="225"/>
       <c r="E5" s="170">
         <f>'[5]PBX Return Data'!X30</f>
         <v>15598</v>
@@ -28853,7 +28862,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="92"/>
       <c r="N5" s="23" t="s">
-        <v>109</v>
+        <v>311</v>
       </c>
       <c r="O5" s="98">
         <v>0.60271947082721977</v>
@@ -28863,7 +28872,7 @@
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1">
       <c r="B6" s="14"/>
-      <c r="C6" s="221" t="s">
+      <c r="C6" s="226" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="172" t="str">
@@ -28888,7 +28897,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="92"/>
       <c r="N6" s="79" t="s">
-        <v>110</v>
+        <v>312</v>
       </c>
       <c r="O6" s="98">
         <v>0.36156680850201106</v>
@@ -28898,7 +28907,7 @@
     </row>
     <row r="7" spans="2:17" ht="15" customHeight="1">
       <c r="B7" s="14"/>
-      <c r="C7" s="222"/>
+      <c r="C7" s="227"/>
       <c r="D7" s="175" t="str">
         <f>E12</f>
         <v>YTD</v>
@@ -28931,7 +28940,7 @@
     </row>
     <row r="8" spans="2:17" ht="15.75" thickBot="1">
       <c r="B8" s="14"/>
-      <c r="C8" s="222"/>
+      <c r="C8" s="227"/>
       <c r="D8" s="175" t="str">
         <f>F12</f>
         <v>1 Year</v>
@@ -28954,7 +28963,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="92"/>
       <c r="N8" s="97" t="s">
-        <v>111</v>
+        <v>313</v>
       </c>
       <c r="O8" s="99">
         <v>8.0961242836639167E-3</v>
@@ -28964,7 +28973,7 @@
     </row>
     <row r="9" spans="2:17">
       <c r="B9" s="14"/>
-      <c r="C9" s="222"/>
+      <c r="C9" s="227"/>
       <c r="D9" s="175" t="str">
         <f>G12</f>
         <v>3 Years</v>
@@ -28990,7 +28999,7 @@
     </row>
     <row r="10" spans="2:17" ht="15.75" thickBot="1">
       <c r="B10" s="14"/>
-      <c r="C10" s="223"/>
+      <c r="C10" s="228"/>
       <c r="D10" s="178" t="str">
         <f>H12</f>
         <v>Inception*</v>
@@ -29249,14 +29258,14 @@
     </row>
     <row r="20" spans="2:20" ht="14.45" customHeight="1">
       <c r="B20" s="14"/>
-      <c r="C20" s="224" t="s">
+      <c r="C20" s="214" t="s">
         <v>310</v>
       </c>
-      <c r="D20" s="224"/>
-      <c r="E20" s="224"/>
-      <c r="F20" s="224"/>
-      <c r="G20" s="224"/>
-      <c r="H20" s="224"/>
+      <c r="D20" s="214"/>
+      <c r="E20" s="214"/>
+      <c r="F20" s="214"/>
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
       <c r="I20" s="192"/>
       <c r="J20" s="16"/>
       <c r="L20" s="1"/>
@@ -29418,10 +29427,10 @@
     </row>
     <row r="29" spans="2:20" ht="14.45" customHeight="1">
       <c r="B29" s="14"/>
-      <c r="C29" s="225" t="s">
+      <c r="C29" s="215" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="226"/>
+      <c r="D29" s="216"/>
       <c r="E29" s="140" t="s">
         <v>45</v>
       </c>
@@ -29569,10 +29578,10 @@
       <c r="Q34" s="96"/>
     </row>
     <row r="35" spans="3:17">
-      <c r="C35" s="227" t="s">
+      <c r="C35" s="217" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="228"/>
+      <c r="D35" s="218"/>
       <c r="E35" s="145">
         <f>'[5]PBX Return Data'!X17</f>
         <v>-0.13953311535244467</v>

</xml_diff>